<commit_message>
comitted changes for sprint 1 on 01/22
</commit_message>
<xml_diff>
--- a/Automation/TestData/Tumi.xlsx
+++ b/Automation/TestData/Tumi.xlsx
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1205,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>56</v>
@@ -1429,7 +1429,7 @@
   <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,7 +1697,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
@@ -1721,7 +1721,7 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B6" r:id="rId3"/>
     <hyperlink ref="B7" r:id="rId4" display="Employee.tumi@gmail.com"/>
-    <hyperlink ref="B8" r:id="rId5" display="Employee.tumi@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>